<commit_message>
Correcion en muestreo de datos
</commit_message>
<xml_diff>
--- a/SpaOnline/ModeloDominio/Servicios - Muestreo Datos.xlsx
+++ b/SpaOnline/ModeloDominio/Servicios - Muestreo Datos.xlsx
@@ -8,22 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis ospina\OneDrive\Documentos\GitHub\DOO\SpaOnline\ModeloDominio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1A7ECA-2A38-4927-B2B7-421DB733ACBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46799591-2D47-4459-BD8D-8A50CC2251E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="6" xr2:uid="{9AD29915-CB49-430C-A10E-F60FF2C9A65A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="2" activeTab="9" xr2:uid="{9AD29915-CB49-430C-A10E-F60FF2C9A65A}"/>
   </bookViews>
   <sheets>
     <sheet name="Modelo de Dominio Anemico" sheetId="1" r:id="rId1"/>
     <sheet name="Objetos de dominio" sheetId="2" r:id="rId2"/>
     <sheet name="Tarifa" sheetId="10" r:id="rId3"/>
-    <sheet name="TipoServicio" sheetId="6" r:id="rId4"/>
-    <sheet name="Servicio" sheetId="5" r:id="rId5"/>
-    <sheet name="Oferta" sheetId="7" r:id="rId6"/>
-    <sheet name="Evento" sheetId="8" r:id="rId7"/>
-    <sheet name="Cliente" sheetId="9" r:id="rId8"/>
+    <sheet name="Estado" sheetId="13" r:id="rId4"/>
+    <sheet name="TipoServicio" sheetId="6" r:id="rId5"/>
+    <sheet name="Servicio" sheetId="5" r:id="rId6"/>
+    <sheet name="Oferta" sheetId="7" r:id="rId7"/>
+    <sheet name="Evento" sheetId="8" r:id="rId8"/>
+    <sheet name="Cliente" sheetId="9" r:id="rId9"/>
+    <sheet name="Notificaciones" sheetId="11" r:id="rId10"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId9"/>
+    <externalReference r:id="rId11"/>
+    <externalReference r:id="rId12"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -66,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="78">
   <si>
     <t xml:space="preserve">Nombre </t>
   </si>
@@ -149,9 +152,6 @@
     <t>Objeto de dominio que contiene información sobre los tipos de servicios ofrecidos por el spa, como masajes, tratamientos faciales, pedicura.</t>
   </si>
   <si>
-    <t>OfertaPedicuraMadres</t>
-  </si>
-  <si>
     <t>OfertaFacial</t>
   </si>
   <si>
@@ -230,12 +230,6 @@
     <t>Valor</t>
   </si>
   <si>
-    <t>31/02/2024</t>
-  </si>
-  <si>
-    <t>31/04/2024</t>
-  </si>
-  <si>
     <t>Referenciado</t>
   </si>
   <si>
@@ -246,6 +240,69 @@
   </si>
   <si>
     <t>Contexto</t>
+  </si>
+  <si>
+    <t>Objeto de dominio que contiene información sobre los eventos  asociados a las ofertas ofrecidas por el spa</t>
+  </si>
+  <si>
+    <t>TipoNotificacion</t>
+  </si>
+  <si>
+    <t>NotificadoA</t>
+  </si>
+  <si>
+    <t>Mesaje</t>
+  </si>
+  <si>
+    <t>EsNotificado</t>
+  </si>
+  <si>
+    <t>La reserva ha sido realizada exitosamente</t>
+  </si>
+  <si>
+    <t>Queremos informarte que por el mes de madres hay descuento en limpieza facial</t>
+  </si>
+  <si>
+    <t>Le adjuntamos su factura emitida</t>
+  </si>
+  <si>
+    <t>False</t>
+  </si>
+  <si>
+    <t>Estado</t>
+  </si>
+  <si>
+    <t>identificador</t>
+  </si>
+  <si>
+    <t>estado</t>
+  </si>
+  <si>
+    <t>Combinación Unica</t>
+  </si>
+  <si>
+    <t>Activa</t>
+  </si>
+  <si>
+    <t>Inactiva</t>
+  </si>
+  <si>
+    <t>01/01/2024</t>
+  </si>
+  <si>
+    <t>01/01/2025</t>
+  </si>
+  <si>
+    <t>31/12/2024</t>
+  </si>
+  <si>
+    <t>31/12/2025</t>
+  </si>
+  <si>
+    <t>OfertaPedicura</t>
+  </si>
+  <si>
+    <t>Objteto de dominio que contiene información acerca del estado de la tarifa que tendra cada servicio</t>
   </si>
 </sst>
 </file>
@@ -256,7 +313,7 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-[$$-240A]\ * #,##0.00_-;\-[$$-240A]\ * #,##0.00_-;_-[$$-240A]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -301,8 +358,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -321,8 +395,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -345,13 +425,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -384,11 +480,19 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Moneda" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{D30BAD19-9307-41A9-84AE-2383E78F785B}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -413,17 +517,17 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>353431</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>124241</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>611068</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>38743</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Imagen 1">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2339637A-AC4E-09C5-0BC3-E78B386CFFFB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6DA04341-EEA8-2894-80F2-61B8690891B9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -440,7 +544,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="7211431" cy="2981741"/>
+          <a:ext cx="10517068" cy="4610743"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -466,9 +570,9 @@
       <sheetName val="TipoIdentificacion"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
       <sheetData sheetId="3">
         <row r="2">
           <cell r="B2" t="str">
@@ -490,6 +594,65 @@
         <row r="9">
           <cell r="B9" t="str">
             <v>TI</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Modelo de Dominio Anemico"/>
+      <sheetName val="Objetos de dominio"/>
+      <sheetName val="Notificación"/>
+      <sheetName val="Cliente"/>
+      <sheetName val="TipoNotificación"/>
+      <sheetName val="ListaNotificacion"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3">
+        <row r="2">
+          <cell r="G2" t="str">
+            <v>martina.corrales@gmail.com</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="G4" t="str">
+            <v>lucrecia.gomez@hotmail.com</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="4">
+        <row r="2">
+          <cell r="B2" t="str">
+            <v>Reserva</v>
+          </cell>
+        </row>
+        <row r="3">
+          <cell r="B3" t="str">
+            <v>Evento</v>
+          </cell>
+        </row>
+        <row r="4">
+          <cell r="B4" t="str">
+            <v>Factura</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="5">
+        <row r="2">
+          <cell r="B2" t="str">
+            <v>General</v>
           </cell>
         </row>
       </sheetData>
@@ -833,8 +996,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA198BEE-AB41-4447-8B76-5672FB9C01F4}">
   <dimension ref="L11:N14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -854,12 +1017,108 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6FC7885-849D-49E7-BA65-5E135F92B198}">
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="42.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="21" t="str">
+        <f>+[2]TipoNotificación!B2</f>
+        <v>Reserva</v>
+      </c>
+      <c r="C2" s="1" t="str">
+        <f>[2]Cliente!G2</f>
+        <v>martina.corrales@gmail.com</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="21" t="str">
+        <f>+[2]TipoNotificación!B3</f>
+        <v>Evento</v>
+      </c>
+      <c r="C3" s="1" t="str">
+        <f>+[2]ListaNotificacion!B2</f>
+        <v>General</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="21" t="str">
+        <f>+[2]TipoNotificación!B4</f>
+        <v>Factura</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f>[2]Cliente!G4</f>
+        <v>lucrecia.gomez@hotmail.com</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07D92343-C7F8-498A-9249-704487594109}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,7 +1141,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -929,10 +1188,10 @@
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>3</v>
@@ -941,27 +1200,56 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>57</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>56</v>
+        <v>3</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>58</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" location="Servicio!A1" display="Servicio" xr:uid="{1B941AE0-B9D5-48EA-8B5E-FCA1F99F1D33}"/>
     <hyperlink ref="A3" location="TipoServicio!A1" display="TipoServicio" xr:uid="{C435E2E8-31E6-43EA-8AEA-9447A4E0C810}"/>
-    <hyperlink ref="A5" location="Oferta!A1" display="Oferta" xr:uid="{D7A38285-3128-4507-809F-00E78B181BAE}"/>
+    <hyperlink ref="A7" location="Tarifa!A1" display="Tarifa" xr:uid="{D7A38285-3128-4507-809F-00E78B181BAE}"/>
     <hyperlink ref="A4" location="Oferta!A1" display="Oferta" xr:uid="{11CD3424-938B-4DCF-883F-24E828B8E80C}"/>
-    <hyperlink ref="A6" location="Oferta!A1" display="Oferta" xr:uid="{9A0353DE-577D-4E3E-AAE3-5D3785183622}"/>
+    <hyperlink ref="A8" location="Oferta!A1" display="Oferta" xr:uid="{9A0353DE-577D-4E3E-AAE3-5D3785183622}"/>
+    <hyperlink ref="A6" location="Evento!A1" display="Evento" xr:uid="{ABD1896B-9B8C-47E8-85DE-DB596FF2C733}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -970,29 +1258,30 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357E7923-E7EF-4AD9-A356-C9D474204FF8}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="54" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>53</v>
+        <v>6</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
+        <v>52</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>17</v>
@@ -1000,89 +1289,236 @@
       <c r="E1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="11">
-        <v>100000</v>
-      </c>
-      <c r="C2" s="11" t="str">
+      <c r="B2" s="1" t="str">
         <f>Servicio!B2</f>
         <v>Pedicura Spa</v>
       </c>
-      <c r="D2" s="13">
-        <v>45323</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" s="4" t="str">
-        <f>B2&amp;"-"&amp;C2</f>
-        <v>100000-Pedicura Spa</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C2" s="11">
+        <v>100000</v>
+      </c>
+      <c r="D2" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" s="25" t="str">
+        <f>Estado!$B$2</f>
+        <v>Activa</v>
+      </c>
+      <c r="G2" s="20" t="str">
+        <f>B2&amp;"-"&amp;C2&amp;"-"&amp;D2&amp;"-"&amp;E2</f>
+        <v>Pedicura Spa-100000-01/01/2024-31/12/2024</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="11">
-        <v>120000</v>
-      </c>
-      <c r="C3" s="11" t="str">
+      <c r="B3" s="1" t="str">
         <f>Servicio!B3</f>
         <v>Tratamiento Facial Antiedad</v>
       </c>
-      <c r="D3" s="13">
-        <v>45323</v>
-      </c>
-      <c r="E3" s="13">
-        <v>45382</v>
-      </c>
-      <c r="F3" s="4" t="str">
-        <f t="shared" ref="F3:F4" si="0">B3&amp;"-"&amp;C3</f>
-        <v>120000-Tratamiento Facial Antiedad</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="11">
+        <v>120000</v>
+      </c>
+      <c r="D3" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="25" t="str">
+        <f>Estado!$B$2</f>
+        <v>Activa</v>
+      </c>
+      <c r="G3" s="20" t="str">
+        <f t="shared" ref="G3:G7" si="0">B3&amp;"-"&amp;C3&amp;"-"&amp;D3&amp;"-"&amp;E3</f>
+        <v>Tratamiento Facial Antiedad-120000-01/01/2024-31/12/2024</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="11">
-        <v>100000</v>
-      </c>
-      <c r="C4" s="11" t="str">
+      <c r="B4" s="1" t="str">
         <f>Servicio!B4</f>
         <v>Masaje Relajante</v>
       </c>
-      <c r="D4" s="13">
-        <v>45323</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" s="4" t="str">
+      <c r="C4" s="11">
+        <v>150000</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="25" t="str">
+        <f>Estado!$B$2</f>
+        <v>Activa</v>
+      </c>
+      <c r="G4" s="20" t="str">
         <f t="shared" si="0"/>
-        <v>100000-Masaje Relajante</v>
+        <v>Masaje Relajante-150000-01/01/2024-31/12/2024</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="str">
+        <f>Servicio!B2</f>
+        <v>Pedicura Spa</v>
+      </c>
+      <c r="C5" s="11">
+        <v>200000</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" s="25" t="str">
+        <f>Estado!$B$3</f>
+        <v>Inactiva</v>
+      </c>
+      <c r="G5" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Pedicura Spa-200000-01/01/2025-31/12/2025</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="str">
+        <f>Servicio!B3</f>
+        <v>Tratamiento Facial Antiedad</v>
+      </c>
+      <c r="C6" s="11">
+        <v>180000</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="25" t="str">
+        <f>Estado!$B$3</f>
+        <v>Inactiva</v>
+      </c>
+      <c r="G6" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Tratamiento Facial Antiedad-180000-01/01/2025-31/12/2025</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="str">
+        <f>Servicio!B4</f>
+        <v>Masaje Relajante</v>
+      </c>
+      <c r="C7" s="11">
+        <v>220000</v>
+      </c>
+      <c r="D7" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" s="25" t="str">
+        <f>Estado!$B$3</f>
+        <v>Inactiva</v>
+      </c>
+      <c r="G7" s="20" t="str">
+        <f t="shared" si="0"/>
+        <v>Masaje Relajante-220000-01/01/2025-31/12/2025</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="F2" location="Estado!B2" display="activo" xr:uid="{6F6830C8-CC05-46F8-94BC-E84B5A393DB7}"/>
+    <hyperlink ref="F3:F4" location="Estado!B2" display="activo" xr:uid="{C13B0E0A-2695-4555-8C46-C00CD62D2D76}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB0FF228-A94B-46E3-A75E-16170844C9F2}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="22">
+        <v>1</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" s="22" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="22">
+        <v>2</v>
+      </c>
+      <c r="B3" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>71</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DD65F79-6C02-4D3F-86AD-E8559480B117}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1143,12 +1579,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{952BDDC5-1485-4BC4-A31B-18839936F54D}">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1175,7 +1611,7 @@
         <v>12</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>5</v>
@@ -1189,14 +1625,14 @@
         <v>15</v>
       </c>
       <c r="C2" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2" s="10" t="str">
         <f>TipoServicio!C2</f>
         <v>Pedicura y Manicura</v>
       </c>
       <c r="E2" s="18">
-        <f>Tarifa!B2</f>
+        <f>Tarifa!C2</f>
         <v>100000</v>
       </c>
       <c r="F2" s="4" t="str">
@@ -1212,14 +1648,14 @@
         <v>14</v>
       </c>
       <c r="C3" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D3" s="10" t="str">
         <f>TipoServicio!C3</f>
         <v>Tratamiento Facial</v>
       </c>
       <c r="E3" s="18">
-        <f>Tarifa!B3</f>
+        <f>Tarifa!C3</f>
         <v>120000</v>
       </c>
       <c r="F3" s="4" t="str">
@@ -1235,15 +1671,15 @@
         <v>13</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="10" t="str">
         <f>TipoServicio!C4</f>
         <v>Masaje</v>
       </c>
       <c r="E4" s="18">
-        <f>Tarifa!B4</f>
-        <v>100000</v>
+        <f>Tarifa!C4</f>
+        <v>150000</v>
       </c>
       <c r="F4" s="4" t="str">
         <f t="shared" si="0"/>
@@ -1265,12 +1701,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62648864-EB04-44C3-BA83-B67C2DB45844}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1280,11 +1716,10 @@
     <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
@@ -1298,10 +1733,10 @@
         <v>16</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>17</v>
@@ -1309,19 +1744,16 @@
       <c r="H1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>76</v>
       </c>
       <c r="C2" s="10" t="str">
         <f>Servicio!B2</f>
@@ -1344,21 +1776,17 @@
       <c r="H2" s="13">
         <v>45402</v>
       </c>
-      <c r="I2" s="1" t="str">
-        <f>Evento!B2</f>
-        <v>OfertaPedicura Madres</v>
-      </c>
-      <c r="J2" s="4" t="str">
+      <c r="I2" s="4" t="str">
         <f>B2&amp;" "&amp;D2</f>
-        <v>OfertaPedicuraMadres 0,2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>OfertaPedicura 0,2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="10" t="str">
         <f>Servicio!B3</f>
@@ -1381,21 +1809,17 @@
       <c r="H3" s="13">
         <v>45403</v>
       </c>
-      <c r="I3" s="1" t="str">
-        <f>Evento!B3</f>
-        <v>OfertaFacial San Valentin</v>
-      </c>
-      <c r="J3" s="4" t="str">
-        <f t="shared" ref="J3:J4" si="1">B3&amp;" "&amp;D3</f>
+      <c r="I3" s="4" t="str">
+        <f t="shared" ref="I3:I4" si="1">B3&amp;" "&amp;D3</f>
         <v>OfertaFacial 0,25</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" s="10" t="str">
         <f>Servicio!B4</f>
@@ -1406,11 +1830,11 @@
       </c>
       <c r="E4" s="19">
         <f>Servicio!E4</f>
-        <v>100000</v>
+        <v>150000</v>
       </c>
       <c r="F4" s="19">
         <f>E4-(E4*D4)</f>
-        <v>85000</v>
+        <v>127500</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>21</v>
@@ -1418,17 +1842,13 @@
       <c r="H4" s="13">
         <v>45404</v>
       </c>
-      <c r="I4" s="1" t="str">
-        <f>Evento!B4</f>
-        <v>OfertaMasaje Black Friday</v>
-      </c>
-      <c r="J4" s="4" t="str">
+      <c r="I4" s="4" t="str">
         <f t="shared" si="1"/>
         <v>OfertaMasaje 0,15</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="J10" s="15"/>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I10" s="15"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1440,92 +1860,117 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21DB1D5A-5E80-4FAF-B6D3-9725EF96B51E}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.28515625" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>31</v>
+      <c r="B2" s="10" t="str">
+        <f>Oferta!B2</f>
+        <v>OfertaPedicura</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" s="4" t="str">
-        <f>B2</f>
+        <v>30</v>
+      </c>
+      <c r="D2" s="10" t="str">
+        <f>Notificaciones!$C$3</f>
+        <v>General</v>
+      </c>
+      <c r="E2" s="4" t="str">
+        <f>C2</f>
         <v>OfertaPedicura Madres</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>32</v>
+      <c r="B3" s="10" t="str">
+        <f>Oferta!B3</f>
+        <v>OfertaFacial</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D3" s="4" t="str">
-        <f t="shared" ref="D3:D4" si="0">B3</f>
+        <v>31</v>
+      </c>
+      <c r="D3" s="10" t="str">
+        <f>Notificaciones!$C$3</f>
+        <v>General</v>
+      </c>
+      <c r="E3" s="4" t="str">
+        <f t="shared" ref="E3:E4" si="0">C3</f>
         <v>OfertaFacial San Valentin</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>33</v>
+      <c r="B4" s="10" t="str">
+        <f>Oferta!B4</f>
+        <v>OfertaMasaje</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="D4" s="4" t="str">
+        <v>32</v>
+      </c>
+      <c r="D4" s="10" t="str">
+        <f>Notificaciones!$C$3</f>
+        <v>General</v>
+      </c>
+      <c r="E4" s="4" t="str">
         <f t="shared" si="0"/>
         <v>OfertaMasaje Black Friday</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" location="Notificaciones!A1" display="Notificaciones!A1" xr:uid="{2708A9D5-D92A-4B65-8C66-B36792AC6228}"/>
+    <hyperlink ref="B2" location="Oferta!B2" display="Oferta!B2" xr:uid="{0349CDC5-8CAD-45D5-8487-032E349C1F24}"/>
+    <hyperlink ref="B3:B4" location="Oferta!B2" display="Oferta!B2" xr:uid="{9FA7C2A0-21FD-4377-BF5F-583851742314}"/>
+    <hyperlink ref="D3:D4" location="Notificaciones!A1" display="Notificaciones!A1" xr:uid="{9FF8EDAD-A7B1-420A-B1C8-087BF8371DD8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C48326-81E7-4BC0-9589-6DD184028A22}">
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1544,19 +1989,19 @@
         <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>5</v>
@@ -1567,7 +2012,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2" s="1" t="str">
         <f>+[1]TipoIdentificacion!B7</f>
@@ -1580,7 +2025,7 @@
         <v>3116987523</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G2" s="4" t="str">
         <f>+B2&amp;"-"&amp;D2</f>
@@ -1592,7 +2037,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C3" s="1" t="str">
         <f>+[1]TipoIdentificacion!B8</f>
@@ -1605,7 +2050,7 @@
         <v>3639874520</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G3" s="4" t="str">
         <f t="shared" ref="G3:G4" si="0">+B3&amp;"-"&amp;D3</f>
@@ -1617,7 +2062,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="1" t="str">
         <f>+[1]TipoIdentificacion!B9</f>
@@ -1630,7 +2075,7 @@
         <v>3793175677</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G4" s="4" t="str">
         <f t="shared" si="0"/>

</xml_diff>